<commit_message>
refactor(ddd): DDD refactor big changed!!!
</commit_message>
<xml_diff>
--- a/examples/points.xlsx
+++ b/examples/points.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="33">
   <si>
     <t>device_code</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>水阀开度设定</t>
+  </si>
+  <si>
+    <t>AHU_2_2</t>
   </si>
 </sst>
 </file>
@@ -1279,10 +1282,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="6"/>
@@ -1550,6 +1553,236 @@
         <v>31</v>
       </c>
     </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2">
+        <v>833</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>60</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2">
+        <v>833</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>60</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2">
+        <v>833</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>60</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2">
+        <v>833</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2">
+        <v>60</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="2">
+        <v>833</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="2">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2">
+        <v>60</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="2">
+        <v>833</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="2">
+        <v>6</v>
+      </c>
+      <c r="F17" s="2">
+        <v>60</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2">
+        <v>833</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="2">
+        <v>7</v>
+      </c>
+      <c r="F18" s="2">
+        <v>60</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2">
+        <v>833</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>60</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2">
+        <v>833</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>60</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="2">
+        <v>833</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <v>60</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>